<commit_message>
Works fine for Aditya Birla BL (Sol Prop)
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,22 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Config Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4147C9EA-602E-4C49-A9FF-5FE520780E92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9576307C-0E30-4C42-8D13-9BEEC956974B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="fromtenure" sheetId="4" r:id="rId1"/>
-    <sheet name="dropdown" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet" sheetId="2" r:id="rId3"/>
-    <sheet name="config" sheetId="3" r:id="rId4"/>
+    <sheet name="dropdown" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="2" r:id="rId2"/>
+    <sheet name="config" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2380" uniqueCount="775">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1732" uniqueCount="775">
   <si>
     <t>Secured Loan</t>
   </si>
@@ -2720,3639 +2719,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D61A36B0-7E78-44C0-9139-D42C7076F185}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:AK336"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="41.86328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="41.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="68" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="54" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="77.265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="42.59765625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="51.86328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="55.73046875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.3984375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.59765625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="50.1328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="41.3984375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="53.73046875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="42" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="34.59765625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="40.1328125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="47.265625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="49.73046875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="61.73046875" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="63.3984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="64.86328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="66.73046875" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="47.73046875" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="53.1328125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="73.265625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="68" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="70" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="63.86328125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="65.1328125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="71.1328125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="72.3984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="74.265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="66" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:37" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
-        <v>665</v>
-      </c>
-      <c r="B1" t="s">
-        <v>667</v>
-      </c>
-      <c r="C1" t="s">
-        <v>667</v>
-      </c>
-      <c r="D1" t="s">
-        <v>669</v>
-      </c>
-      <c r="E1" t="s">
-        <v>670</v>
-      </c>
-      <c r="F1" t="s">
-        <v>671</v>
-      </c>
-      <c r="G1" t="s">
-        <v>672</v>
-      </c>
-      <c r="H1" t="s">
-        <v>673</v>
-      </c>
-      <c r="I1" t="s">
-        <v>674</v>
-      </c>
-      <c r="J1" t="s">
-        <v>675</v>
-      </c>
-      <c r="K1" t="s">
-        <v>680</v>
-      </c>
-      <c r="L1" t="s">
-        <v>681</v>
-      </c>
-      <c r="M1" t="s">
-        <v>684</v>
-      </c>
-      <c r="N1" t="s">
-        <v>687</v>
-      </c>
-      <c r="O1" t="s">
-        <v>688</v>
-      </c>
-      <c r="P1" t="s">
-        <v>690</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>694</v>
-      </c>
-      <c r="R1" t="s">
-        <v>697</v>
-      </c>
-      <c r="S1" t="s">
-        <v>698</v>
-      </c>
-      <c r="T1" t="s">
-        <v>699</v>
-      </c>
-      <c r="U1" t="s">
-        <v>700</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>701</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>702</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>703</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>704</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>705</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>707</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>713</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>719</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>720</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>721</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>723</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>724</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>725</v>
-      </c>
-      <c r="AI1" s="2" t="s">
-        <v>727</v>
-      </c>
-      <c r="AJ1" s="2" t="s">
-        <v>728</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>729</v>
-      </c>
-    </row>
-    <row r="2" spans="1:37" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L2" t="s">
-        <v>17</v>
-      </c>
-      <c r="M2" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O2" t="s">
-        <v>20</v>
-      </c>
-      <c r="P2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>21</v>
-      </c>
-      <c r="R2" t="s">
-        <v>19</v>
-      </c>
-      <c r="S2" t="s">
-        <v>21</v>
-      </c>
-      <c r="T2" t="s">
-        <v>22</v>
-      </c>
-      <c r="U2" t="s">
-        <v>23</v>
-      </c>
-      <c r="V2" s="1">
-        <v>0</v>
-      </c>
-      <c r="W2" s="1">
-        <v>0</v>
-      </c>
-      <c r="X2" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y2" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>25</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>9</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>18</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>28</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AI2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:37" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H3" t="s">
-        <v>44</v>
-      </c>
-      <c r="I3" t="s">
-        <v>44</v>
-      </c>
-      <c r="J3" t="s">
-        <v>44</v>
-      </c>
-      <c r="K3" t="s">
-        <v>45</v>
-      </c>
-      <c r="L3" t="s">
-        <v>46</v>
-      </c>
-      <c r="M3" t="s">
-        <v>47</v>
-      </c>
-      <c r="N3" t="s">
-        <v>48</v>
-      </c>
-      <c r="O3" t="s">
-        <v>49</v>
-      </c>
-      <c r="P3" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>50</v>
-      </c>
-      <c r="R3" t="s">
-        <v>48</v>
-      </c>
-      <c r="S3" t="s">
-        <v>50</v>
-      </c>
-      <c r="T3" t="s">
-        <v>51</v>
-      </c>
-      <c r="U3" t="s">
-        <v>52</v>
-      </c>
-      <c r="V3" s="1">
-        <v>1</v>
-      </c>
-      <c r="W3" s="1">
-        <v>1</v>
-      </c>
-      <c r="X3" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y3" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>53</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>54</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>54</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>39</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>47</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>55</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>56</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>57</v>
-      </c>
-      <c r="AI3" s="1">
-        <v>1</v>
-      </c>
-      <c r="AJ3" s="1">
-        <v>1</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:37" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G4" t="s">
-        <v>68</v>
-      </c>
-      <c r="H4" t="s">
-        <v>69</v>
-      </c>
-      <c r="I4" t="s">
-        <v>69</v>
-      </c>
-      <c r="J4" t="s">
-        <v>69</v>
-      </c>
-      <c r="K4" t="s">
-        <v>70</v>
-      </c>
-      <c r="L4" t="s">
-        <v>71</v>
-      </c>
-      <c r="M4" t="s">
-        <v>72</v>
-      </c>
-      <c r="N4" t="s">
-        <v>70</v>
-      </c>
-      <c r="O4" t="s">
-        <v>73</v>
-      </c>
-      <c r="P4" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>74</v>
-      </c>
-      <c r="R4" t="s">
-        <v>70</v>
-      </c>
-      <c r="S4" t="s">
-        <v>74</v>
-      </c>
-      <c r="T4" t="s">
-        <v>75</v>
-      </c>
-      <c r="U4" t="s">
-        <v>76</v>
-      </c>
-      <c r="V4" s="1">
-        <v>2</v>
-      </c>
-      <c r="W4" s="1">
-        <v>2</v>
-      </c>
-      <c r="X4" s="1">
-        <v>2</v>
-      </c>
-      <c r="Y4" s="1">
-        <v>2</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>77</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>77</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>72</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>78</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>79</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>80</v>
-      </c>
-      <c r="AI4" s="1">
-        <v>2</v>
-      </c>
-      <c r="AJ4" s="1">
-        <v>2</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:37" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>88</v>
-      </c>
-      <c r="E5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F5" t="s">
-        <v>90</v>
-      </c>
-      <c r="G5" t="s">
-        <v>91</v>
-      </c>
-      <c r="H5" t="s">
-        <v>92</v>
-      </c>
-      <c r="I5" t="s">
-        <v>92</v>
-      </c>
-      <c r="J5" t="s">
-        <v>92</v>
-      </c>
-      <c r="L5" t="s">
-        <v>93</v>
-      </c>
-      <c r="N5" t="s">
-        <v>54</v>
-      </c>
-      <c r="P5" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>94</v>
-      </c>
-      <c r="R5" t="s">
-        <v>54</v>
-      </c>
-      <c r="S5" t="s">
-        <v>94</v>
-      </c>
-      <c r="T5" t="s">
-        <v>95</v>
-      </c>
-      <c r="V5" s="1">
-        <v>3</v>
-      </c>
-      <c r="W5" s="1">
-        <v>3</v>
-      </c>
-      <c r="X5" s="1">
-        <v>3</v>
-      </c>
-      <c r="Y5" s="1">
-        <v>3</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>96</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>96</v>
-      </c>
-      <c r="AG5" t="s">
-        <v>97</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>98</v>
-      </c>
-      <c r="AI5" s="1">
-        <v>3</v>
-      </c>
-      <c r="AJ5" s="1">
-        <v>3</v>
-      </c>
-      <c r="AK5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="6" spans="1:37" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>105</v>
-      </c>
-      <c r="E6" t="s">
-        <v>106</v>
-      </c>
-      <c r="F6" t="s">
-        <v>107</v>
-      </c>
-      <c r="G6" t="s">
-        <v>108</v>
-      </c>
-      <c r="H6" t="s">
-        <v>109</v>
-      </c>
-      <c r="I6" t="s">
-        <v>109</v>
-      </c>
-      <c r="J6" t="s">
-        <v>109</v>
-      </c>
-      <c r="L6" t="s">
-        <v>110</v>
-      </c>
-      <c r="N6" t="s">
-        <v>111</v>
-      </c>
-      <c r="P6" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>112</v>
-      </c>
-      <c r="R6" t="s">
-        <v>111</v>
-      </c>
-      <c r="S6" t="s">
-        <v>112</v>
-      </c>
-      <c r="T6" t="s">
-        <v>113</v>
-      </c>
-      <c r="V6" s="1">
-        <v>4</v>
-      </c>
-      <c r="W6" s="1">
-        <v>4</v>
-      </c>
-      <c r="X6" s="1">
-        <v>4</v>
-      </c>
-      <c r="Y6" s="1">
-        <v>4</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>114</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>114</v>
-      </c>
-      <c r="AG6" t="s">
-        <v>115</v>
-      </c>
-      <c r="AH6" t="s">
-        <v>116</v>
-      </c>
-      <c r="AI6" s="1">
-        <v>4</v>
-      </c>
-      <c r="AJ6" s="1">
-        <v>4</v>
-      </c>
-      <c r="AK6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="7" spans="1:37" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="D7" t="s">
-        <v>123</v>
-      </c>
-      <c r="E7" t="s">
-        <v>124</v>
-      </c>
-      <c r="F7" t="s">
-        <v>125</v>
-      </c>
-      <c r="G7" t="s">
-        <v>126</v>
-      </c>
-      <c r="H7" t="s">
-        <v>127</v>
-      </c>
-      <c r="I7" t="s">
-        <v>127</v>
-      </c>
-      <c r="J7" t="s">
-        <v>127</v>
-      </c>
-      <c r="P7" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>128</v>
-      </c>
-      <c r="S7" t="s">
-        <v>128</v>
-      </c>
-      <c r="T7" t="s">
-        <v>129</v>
-      </c>
-      <c r="V7" s="1">
-        <v>5</v>
-      </c>
-      <c r="W7" s="1">
-        <v>5</v>
-      </c>
-      <c r="X7" s="1">
-        <v>5</v>
-      </c>
-      <c r="Y7" s="1">
-        <v>5</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>130</v>
-      </c>
-      <c r="AB7" t="s">
-        <v>130</v>
-      </c>
-      <c r="AG7" t="s">
-        <v>70</v>
-      </c>
-      <c r="AH7" t="s">
-        <v>131</v>
-      </c>
-      <c r="AI7" s="1">
-        <v>5</v>
-      </c>
-      <c r="AJ7" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:37" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="D8" t="s">
-        <v>137</v>
-      </c>
-      <c r="E8" t="s">
-        <v>138</v>
-      </c>
-      <c r="F8" t="s">
-        <v>139</v>
-      </c>
-      <c r="G8" t="s">
-        <v>140</v>
-      </c>
-      <c r="P8" t="s">
-        <v>141</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>141</v>
-      </c>
-      <c r="S8" t="s">
-        <v>141</v>
-      </c>
-      <c r="T8" t="s">
-        <v>142</v>
-      </c>
-      <c r="V8" s="1">
-        <v>6</v>
-      </c>
-      <c r="W8" s="1">
-        <v>6</v>
-      </c>
-      <c r="X8" s="1">
-        <v>6</v>
-      </c>
-      <c r="Y8" s="1">
-        <v>6</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>143</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>143</v>
-      </c>
-      <c r="AH8" t="s">
-        <v>10</v>
-      </c>
-      <c r="AI8" s="1">
-        <v>6</v>
-      </c>
-      <c r="AJ8" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:37" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="D9" t="s">
-        <v>146</v>
-      </c>
-      <c r="E9" t="s">
-        <v>147</v>
-      </c>
-      <c r="F9" t="s">
-        <v>148</v>
-      </c>
-      <c r="G9" t="s">
-        <v>149</v>
-      </c>
-      <c r="P9" t="s">
-        <v>150</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>150</v>
-      </c>
-      <c r="S9" t="s">
-        <v>150</v>
-      </c>
-      <c r="V9" s="1">
-        <v>7</v>
-      </c>
-      <c r="W9" s="1">
-        <v>7</v>
-      </c>
-      <c r="X9" s="1">
-        <v>7</v>
-      </c>
-      <c r="Y9" s="1">
-        <v>7</v>
-      </c>
-      <c r="AH9" t="s">
-        <v>151</v>
-      </c>
-      <c r="AI9" s="1">
-        <v>7</v>
-      </c>
-      <c r="AJ9" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:37" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="D10" t="s">
-        <v>154</v>
-      </c>
-      <c r="E10" t="s">
-        <v>155</v>
-      </c>
-      <c r="F10" t="s">
-        <v>156</v>
-      </c>
-      <c r="G10" t="s">
-        <v>157</v>
-      </c>
-      <c r="P10" t="s">
-        <v>158</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>158</v>
-      </c>
-      <c r="S10" t="s">
-        <v>158</v>
-      </c>
-      <c r="V10" s="1">
-        <v>8</v>
-      </c>
-      <c r="W10" s="1">
-        <v>8</v>
-      </c>
-      <c r="X10" s="1">
-        <v>8</v>
-      </c>
-      <c r="Y10" s="1">
-        <v>8</v>
-      </c>
-      <c r="AH10" t="s">
-        <v>159</v>
-      </c>
-      <c r="AI10" s="1">
-        <v>8</v>
-      </c>
-      <c r="AJ10" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:37" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="D11" t="s">
-        <v>161</v>
-      </c>
-      <c r="E11" t="s">
-        <v>162</v>
-      </c>
-      <c r="F11" t="s">
-        <v>163</v>
-      </c>
-      <c r="G11" t="s">
-        <v>164</v>
-      </c>
-      <c r="P11" t="s">
-        <v>165</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>165</v>
-      </c>
-      <c r="S11" t="s">
-        <v>165</v>
-      </c>
-      <c r="V11" s="1">
-        <v>9</v>
-      </c>
-      <c r="W11" s="1">
-        <v>9</v>
-      </c>
-      <c r="X11" s="1">
-        <v>9</v>
-      </c>
-      <c r="Y11" s="1">
-        <v>9</v>
-      </c>
-      <c r="AH11" t="s">
-        <v>166</v>
-      </c>
-      <c r="AI11" s="1">
-        <v>9</v>
-      </c>
-      <c r="AJ11" s="1">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:37" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="1">
-        <v>11</v>
-      </c>
-      <c r="D12" t="s">
-        <v>169</v>
-      </c>
-      <c r="E12" t="s">
-        <v>170</v>
-      </c>
-      <c r="F12" t="s">
-        <v>171</v>
-      </c>
-      <c r="G12" t="s">
-        <v>172</v>
-      </c>
-      <c r="P12" t="s">
-        <v>173</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>173</v>
-      </c>
-      <c r="S12" t="s">
-        <v>173</v>
-      </c>
-      <c r="V12" s="1">
-        <v>10</v>
-      </c>
-      <c r="W12" s="1">
-        <v>10</v>
-      </c>
-      <c r="X12" s="1">
-        <v>10</v>
-      </c>
-      <c r="Y12" s="1">
-        <v>10</v>
-      </c>
-      <c r="AH12" t="s">
-        <v>174</v>
-      </c>
-      <c r="AI12" s="1">
-        <v>10</v>
-      </c>
-      <c r="AJ12" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:37" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="1">
-        <v>12</v>
-      </c>
-      <c r="D13" t="s">
-        <v>177</v>
-      </c>
-      <c r="E13" t="s">
-        <v>178</v>
-      </c>
-      <c r="F13" t="s">
-        <v>179</v>
-      </c>
-      <c r="G13" t="s">
-        <v>180</v>
-      </c>
-      <c r="P13" t="s">
-        <v>181</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>181</v>
-      </c>
-      <c r="S13" t="s">
-        <v>181</v>
-      </c>
-      <c r="V13" s="1">
-        <v>11</v>
-      </c>
-      <c r="W13" s="1">
-        <v>11</v>
-      </c>
-      <c r="X13" s="1">
-        <v>11</v>
-      </c>
-      <c r="Y13" s="1">
-        <v>11</v>
-      </c>
-      <c r="AH13" t="s">
-        <v>182</v>
-      </c>
-      <c r="AI13" s="1">
-        <v>11</v>
-      </c>
-      <c r="AJ13" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:37" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="1">
-        <v>13</v>
-      </c>
-      <c r="D14" t="s">
-        <v>185</v>
-      </c>
-      <c r="E14" t="s">
-        <v>186</v>
-      </c>
-      <c r="F14" t="s">
-        <v>187</v>
-      </c>
-      <c r="G14" t="s">
-        <v>188</v>
-      </c>
-      <c r="P14" t="s">
-        <v>189</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>189</v>
-      </c>
-      <c r="S14" t="s">
-        <v>189</v>
-      </c>
-      <c r="V14" s="1">
-        <v>12</v>
-      </c>
-      <c r="X14" s="1">
-        <v>12</v>
-      </c>
-      <c r="AH14" t="s">
-        <v>190</v>
-      </c>
-      <c r="AI14" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:37" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="1">
-        <v>14</v>
-      </c>
-      <c r="D15" t="s">
-        <v>193</v>
-      </c>
-      <c r="E15" t="s">
-        <v>194</v>
-      </c>
-      <c r="F15" t="s">
-        <v>195</v>
-      </c>
-      <c r="G15" t="s">
-        <v>196</v>
-      </c>
-      <c r="P15" t="s">
-        <v>197</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>197</v>
-      </c>
-      <c r="S15" t="s">
-        <v>197</v>
-      </c>
-      <c r="V15" s="1">
-        <v>13</v>
-      </c>
-      <c r="X15" s="1">
-        <v>13</v>
-      </c>
-      <c r="AH15" t="s">
-        <v>198</v>
-      </c>
-      <c r="AI15" s="1">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:37" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="1">
-        <v>15</v>
-      </c>
-      <c r="D16" t="s">
-        <v>201</v>
-      </c>
-      <c r="E16" t="s">
-        <v>202</v>
-      </c>
-      <c r="G16" t="s">
-        <v>203</v>
-      </c>
-      <c r="P16" t="s">
-        <v>204</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>204</v>
-      </c>
-      <c r="S16" t="s">
-        <v>204</v>
-      </c>
-      <c r="V16" s="1">
-        <v>14</v>
-      </c>
-      <c r="X16" s="1">
-        <v>14</v>
-      </c>
-      <c r="AH16" t="s">
-        <v>205</v>
-      </c>
-      <c r="AI16" s="1">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="1">
-        <v>16</v>
-      </c>
-      <c r="D17" t="s">
-        <v>208</v>
-      </c>
-      <c r="E17" t="s">
-        <v>209</v>
-      </c>
-      <c r="G17" t="s">
-        <v>210</v>
-      </c>
-      <c r="P17" t="s">
-        <v>211</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>211</v>
-      </c>
-      <c r="S17" t="s">
-        <v>211</v>
-      </c>
-      <c r="V17" s="1">
-        <v>15</v>
-      </c>
-      <c r="X17" s="1">
-        <v>15</v>
-      </c>
-      <c r="AH17" t="s">
-        <v>212</v>
-      </c>
-      <c r="AI17" s="1">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="1">
-        <v>17</v>
-      </c>
-      <c r="D18" t="s">
-        <v>215</v>
-      </c>
-      <c r="E18" t="s">
-        <v>216</v>
-      </c>
-      <c r="P18" t="s">
-        <v>217</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>217</v>
-      </c>
-      <c r="S18" t="s">
-        <v>217</v>
-      </c>
-      <c r="V18" s="1">
-        <v>16</v>
-      </c>
-      <c r="X18" s="1">
-        <v>16</v>
-      </c>
-      <c r="AH18" t="s">
-        <v>70</v>
-      </c>
-      <c r="AI18" s="1">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="1">
-        <v>18</v>
-      </c>
-      <c r="D19" t="s">
-        <v>220</v>
-      </c>
-      <c r="E19" t="s">
-        <v>221</v>
-      </c>
-      <c r="P19" t="s">
-        <v>222</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>222</v>
-      </c>
-      <c r="S19" t="s">
-        <v>222</v>
-      </c>
-      <c r="V19" s="1">
-        <v>17</v>
-      </c>
-      <c r="X19" s="1">
-        <v>17</v>
-      </c>
-      <c r="AH19" t="s">
-        <v>223</v>
-      </c>
-      <c r="AI19" s="1">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="1">
-        <v>19</v>
-      </c>
-      <c r="D20" t="s">
-        <v>226</v>
-      </c>
-      <c r="E20" t="s">
-        <v>227</v>
-      </c>
-      <c r="P20" t="s">
-        <v>228</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>228</v>
-      </c>
-      <c r="S20" t="s">
-        <v>228</v>
-      </c>
-      <c r="V20" s="1">
-        <v>18</v>
-      </c>
-      <c r="X20" s="1">
-        <v>18</v>
-      </c>
-      <c r="AH20" t="s">
-        <v>229</v>
-      </c>
-      <c r="AI20" s="1">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="1">
-        <v>20</v>
-      </c>
-      <c r="D21" t="s">
-        <v>232</v>
-      </c>
-      <c r="E21" t="s">
-        <v>233</v>
-      </c>
-      <c r="P21" t="s">
-        <v>234</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>234</v>
-      </c>
-      <c r="S21" t="s">
-        <v>234</v>
-      </c>
-      <c r="V21" s="1">
-        <v>19</v>
-      </c>
-      <c r="X21" s="1">
-        <v>19</v>
-      </c>
-      <c r="AH21" t="s">
-        <v>235</v>
-      </c>
-      <c r="AI21" s="1">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="1">
-        <v>21</v>
-      </c>
-      <c r="D22" t="s">
-        <v>238</v>
-      </c>
-      <c r="E22" t="s">
-        <v>239</v>
-      </c>
-      <c r="P22" t="s">
-        <v>240</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>240</v>
-      </c>
-      <c r="S22" t="s">
-        <v>240</v>
-      </c>
-      <c r="V22" s="1">
-        <v>20</v>
-      </c>
-      <c r="X22" s="1">
-        <v>20</v>
-      </c>
-      <c r="AH22" t="s">
-        <v>241</v>
-      </c>
-      <c r="AI22" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="1">
-        <v>22</v>
-      </c>
-      <c r="D23" t="s">
-        <v>244</v>
-      </c>
-      <c r="P23" t="s">
-        <v>245</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>245</v>
-      </c>
-      <c r="S23" t="s">
-        <v>245</v>
-      </c>
-      <c r="V23" s="1">
-        <v>21</v>
-      </c>
-      <c r="X23" s="1">
-        <v>21</v>
-      </c>
-      <c r="AH23" t="s">
-        <v>246</v>
-      </c>
-      <c r="AI23" s="1">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="1">
-        <v>23</v>
-      </c>
-      <c r="D24" t="s">
-        <v>249</v>
-      </c>
-      <c r="P24" t="s">
-        <v>250</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>250</v>
-      </c>
-      <c r="S24" t="s">
-        <v>250</v>
-      </c>
-      <c r="V24" s="1">
-        <v>22</v>
-      </c>
-      <c r="X24" s="1">
-        <v>22</v>
-      </c>
-      <c r="AH24" t="s">
-        <v>251</v>
-      </c>
-      <c r="AI24" s="1">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="1">
-        <v>24</v>
-      </c>
-      <c r="D25" t="s">
-        <v>254</v>
-      </c>
-      <c r="P25" t="s">
-        <v>255</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>255</v>
-      </c>
-      <c r="S25" t="s">
-        <v>255</v>
-      </c>
-      <c r="V25" s="1">
-        <v>23</v>
-      </c>
-      <c r="X25" s="1">
-        <v>23</v>
-      </c>
-      <c r="AH25" t="s">
-        <v>256</v>
-      </c>
-      <c r="AI25" s="1">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="1">
-        <v>25</v>
-      </c>
-      <c r="D26" t="s">
-        <v>259</v>
-      </c>
-      <c r="P26" t="s">
-        <v>260</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>260</v>
-      </c>
-      <c r="S26" t="s">
-        <v>260</v>
-      </c>
-      <c r="V26" s="1">
-        <v>24</v>
-      </c>
-      <c r="X26" s="1">
-        <v>24</v>
-      </c>
-      <c r="AH26" t="s">
-        <v>261</v>
-      </c>
-      <c r="AI26" s="1">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="1">
-        <v>26</v>
-      </c>
-      <c r="D27" t="s">
-        <v>264</v>
-      </c>
-      <c r="P27" t="s">
-        <v>265</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>265</v>
-      </c>
-      <c r="S27" t="s">
-        <v>265</v>
-      </c>
-      <c r="V27" s="1">
-        <v>25</v>
-      </c>
-      <c r="X27" s="1">
-        <v>25</v>
-      </c>
-      <c r="AH27" t="s">
-        <v>266</v>
-      </c>
-      <c r="AI27" s="1">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="1">
-        <v>27</v>
-      </c>
-      <c r="D28" t="s">
-        <v>269</v>
-      </c>
-      <c r="P28" t="s">
-        <v>270</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>270</v>
-      </c>
-      <c r="S28" t="s">
-        <v>270</v>
-      </c>
-      <c r="V28" s="1">
-        <v>26</v>
-      </c>
-      <c r="X28" s="1">
-        <v>26</v>
-      </c>
-      <c r="AI28" s="1">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="1">
-        <v>28</v>
-      </c>
-      <c r="D29" t="s">
-        <v>273</v>
-      </c>
-      <c r="P29" t="s">
-        <v>274</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>274</v>
-      </c>
-      <c r="S29" t="s">
-        <v>274</v>
-      </c>
-      <c r="V29" s="1">
-        <v>27</v>
-      </c>
-      <c r="X29" s="1">
-        <v>27</v>
-      </c>
-      <c r="AI29" s="1">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="1">
-        <v>29</v>
-      </c>
-      <c r="D30" t="s">
-        <v>277</v>
-      </c>
-      <c r="P30" t="s">
-        <v>278</v>
-      </c>
-      <c r="Q30" t="s">
-        <v>278</v>
-      </c>
-      <c r="S30" t="s">
-        <v>278</v>
-      </c>
-      <c r="V30" s="1">
-        <v>28</v>
-      </c>
-      <c r="X30" s="1">
-        <v>28</v>
-      </c>
-      <c r="AI30" s="1">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="1">
-        <v>30</v>
-      </c>
-      <c r="D31" t="s">
-        <v>280</v>
-      </c>
-      <c r="P31" t="s">
-        <v>281</v>
-      </c>
-      <c r="Q31" t="s">
-        <v>281</v>
-      </c>
-      <c r="S31" t="s">
-        <v>281</v>
-      </c>
-      <c r="V31" s="1">
-        <v>29</v>
-      </c>
-      <c r="X31" s="1">
-        <v>29</v>
-      </c>
-      <c r="AI31" s="1">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="1">
-        <v>31</v>
-      </c>
-      <c r="D32" t="s">
-        <v>284</v>
-      </c>
-      <c r="P32" t="s">
-        <v>285</v>
-      </c>
-      <c r="Q32" t="s">
-        <v>285</v>
-      </c>
-      <c r="S32" t="s">
-        <v>285</v>
-      </c>
-      <c r="V32" s="1">
-        <v>30</v>
-      </c>
-      <c r="X32" s="1">
-        <v>30</v>
-      </c>
-      <c r="AI32" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="1">
-        <v>32</v>
-      </c>
-      <c r="D33" t="s">
-        <v>288</v>
-      </c>
-      <c r="P33" t="s">
-        <v>289</v>
-      </c>
-      <c r="Q33" t="s">
-        <v>289</v>
-      </c>
-      <c r="S33" t="s">
-        <v>289</v>
-      </c>
-      <c r="V33" s="1">
-        <v>31</v>
-      </c>
-      <c r="X33" s="1">
-        <v>31</v>
-      </c>
-      <c r="AI33" s="1">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="1">
-        <v>33</v>
-      </c>
-      <c r="D34" t="s">
-        <v>291</v>
-      </c>
-      <c r="P34" t="s">
-        <v>292</v>
-      </c>
-      <c r="Q34" t="s">
-        <v>292</v>
-      </c>
-      <c r="S34" t="s">
-        <v>292</v>
-      </c>
-      <c r="V34" s="1">
-        <v>32</v>
-      </c>
-      <c r="X34" s="1">
-        <v>32</v>
-      </c>
-      <c r="AI34" s="1">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="1">
-        <v>34</v>
-      </c>
-      <c r="D35" t="s">
-        <v>295</v>
-      </c>
-      <c r="P35" t="s">
-        <v>296</v>
-      </c>
-      <c r="Q35" t="s">
-        <v>296</v>
-      </c>
-      <c r="S35" t="s">
-        <v>296</v>
-      </c>
-      <c r="V35" s="1">
-        <v>33</v>
-      </c>
-      <c r="X35" s="1">
-        <v>33</v>
-      </c>
-      <c r="AI35" s="1">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="1">
-        <v>35</v>
-      </c>
-      <c r="D36" t="s">
-        <v>298</v>
-      </c>
-      <c r="P36" t="s">
-        <v>299</v>
-      </c>
-      <c r="Q36" t="s">
-        <v>299</v>
-      </c>
-      <c r="S36" t="s">
-        <v>299</v>
-      </c>
-      <c r="V36" s="1">
-        <v>34</v>
-      </c>
-      <c r="X36" s="1">
-        <v>34</v>
-      </c>
-      <c r="AI36" s="1">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="1">
-        <v>36</v>
-      </c>
-      <c r="D37" t="s">
-        <v>301</v>
-      </c>
-      <c r="P37" t="s">
-        <v>302</v>
-      </c>
-      <c r="Q37" t="s">
-        <v>302</v>
-      </c>
-      <c r="S37" t="s">
-        <v>302</v>
-      </c>
-      <c r="V37" s="1">
-        <v>35</v>
-      </c>
-      <c r="X37" s="1">
-        <v>35</v>
-      </c>
-      <c r="AI37" s="1">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="38" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="1">
-        <v>37</v>
-      </c>
-      <c r="D38" t="s">
-        <v>304</v>
-      </c>
-      <c r="V38" s="1">
-        <v>36</v>
-      </c>
-      <c r="X38" s="1">
-        <v>36</v>
-      </c>
-      <c r="AI38" s="1">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="1">
-        <v>38</v>
-      </c>
-      <c r="D39" t="s">
-        <v>306</v>
-      </c>
-      <c r="V39" s="1">
-        <v>37</v>
-      </c>
-      <c r="X39" s="1">
-        <v>37</v>
-      </c>
-      <c r="AI39" s="1">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="40" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="1">
-        <v>39</v>
-      </c>
-      <c r="D40" t="s">
-        <v>308</v>
-      </c>
-      <c r="V40" s="1">
-        <v>38</v>
-      </c>
-      <c r="X40" s="1">
-        <v>38</v>
-      </c>
-      <c r="AI40" s="1">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="41" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="1">
-        <v>40</v>
-      </c>
-      <c r="D41" t="s">
-        <v>310</v>
-      </c>
-      <c r="V41" s="1">
-        <v>39</v>
-      </c>
-      <c r="X41" s="1">
-        <v>39</v>
-      </c>
-      <c r="AI41" s="1">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="42" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="1">
-        <v>41</v>
-      </c>
-      <c r="D42" t="s">
-        <v>312</v>
-      </c>
-      <c r="V42" s="1">
-        <v>40</v>
-      </c>
-      <c r="X42" s="1">
-        <v>40</v>
-      </c>
-      <c r="AI42" s="1">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="43" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A43" s="1">
-        <v>42</v>
-      </c>
-      <c r="D43" t="s">
-        <v>314</v>
-      </c>
-      <c r="V43" s="1">
-        <v>41</v>
-      </c>
-      <c r="X43" s="1">
-        <v>41</v>
-      </c>
-      <c r="AI43" s="1">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="44" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A44" s="1">
-        <v>43</v>
-      </c>
-      <c r="D44" t="s">
-        <v>316</v>
-      </c>
-      <c r="V44" s="1">
-        <v>42</v>
-      </c>
-      <c r="X44" s="1">
-        <v>42</v>
-      </c>
-      <c r="AI44" s="1">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="45" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="1">
-        <v>44</v>
-      </c>
-      <c r="D45" t="s">
-        <v>318</v>
-      </c>
-      <c r="V45" s="1">
-        <v>43</v>
-      </c>
-      <c r="X45" s="1">
-        <v>43</v>
-      </c>
-      <c r="AI45" s="1">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="46" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A46" s="1">
-        <v>45</v>
-      </c>
-      <c r="D46" t="s">
-        <v>320</v>
-      </c>
-      <c r="V46" s="1">
-        <v>44</v>
-      </c>
-      <c r="X46" s="1">
-        <v>44</v>
-      </c>
-      <c r="AI46" s="1">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="47" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="1">
-        <v>46</v>
-      </c>
-      <c r="D47" t="s">
-        <v>322</v>
-      </c>
-      <c r="V47" s="1">
-        <v>45</v>
-      </c>
-      <c r="X47" s="1">
-        <v>45</v>
-      </c>
-      <c r="AI47" s="1">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="48" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="1">
-        <v>47</v>
-      </c>
-      <c r="D48" t="s">
-        <v>324</v>
-      </c>
-      <c r="V48" s="1">
-        <v>46</v>
-      </c>
-      <c r="X48" s="1">
-        <v>46</v>
-      </c>
-      <c r="AI48" s="1">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="49" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="1">
-        <v>48</v>
-      </c>
-      <c r="D49" t="s">
-        <v>326</v>
-      </c>
-      <c r="V49" s="1">
-        <v>47</v>
-      </c>
-      <c r="X49" s="1">
-        <v>47</v>
-      </c>
-      <c r="AI49" s="1">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="50" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A50" s="1">
-        <v>49</v>
-      </c>
-      <c r="D50" t="s">
-        <v>328</v>
-      </c>
-      <c r="V50" s="1">
-        <v>48</v>
-      </c>
-      <c r="X50" s="1">
-        <v>48</v>
-      </c>
-      <c r="AI50" s="1">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="51" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A51" s="1">
-        <v>50</v>
-      </c>
-      <c r="D51" t="s">
-        <v>330</v>
-      </c>
-      <c r="V51" s="1">
-        <v>49</v>
-      </c>
-      <c r="X51" s="1">
-        <v>49</v>
-      </c>
-      <c r="AI51" s="1">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="52" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A52" s="1">
-        <v>51</v>
-      </c>
-      <c r="D52" t="s">
-        <v>332</v>
-      </c>
-      <c r="V52" s="1">
-        <v>50</v>
-      </c>
-      <c r="X52" s="1">
-        <v>50</v>
-      </c>
-      <c r="AI52" s="1">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="53" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A53" s="1">
-        <v>52</v>
-      </c>
-      <c r="D53" t="s">
-        <v>334</v>
-      </c>
-      <c r="V53" s="1">
-        <v>51</v>
-      </c>
-      <c r="X53" s="1">
-        <v>51</v>
-      </c>
-      <c r="AI53" s="1">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="54" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A54" s="1">
-        <v>53</v>
-      </c>
-      <c r="D54" t="s">
-        <v>336</v>
-      </c>
-      <c r="V54" s="1">
-        <v>52</v>
-      </c>
-      <c r="X54" s="1">
-        <v>52</v>
-      </c>
-      <c r="AI54" s="1">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="55" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A55" s="1">
-        <v>54</v>
-      </c>
-      <c r="D55" t="s">
-        <v>338</v>
-      </c>
-      <c r="V55" s="1">
-        <v>53</v>
-      </c>
-      <c r="X55" s="1">
-        <v>53</v>
-      </c>
-      <c r="AI55" s="1">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="56" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A56" s="1">
-        <v>55</v>
-      </c>
-      <c r="D56" t="s">
-        <v>340</v>
-      </c>
-      <c r="V56" s="1">
-        <v>54</v>
-      </c>
-      <c r="X56" s="1">
-        <v>54</v>
-      </c>
-      <c r="AI56" s="1">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="57" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A57" s="1">
-        <v>56</v>
-      </c>
-      <c r="D57" t="s">
-        <v>342</v>
-      </c>
-      <c r="V57" s="1">
-        <v>55</v>
-      </c>
-      <c r="X57" s="1">
-        <v>55</v>
-      </c>
-      <c r="AI57" s="1">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="58" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A58" s="1">
-        <v>57</v>
-      </c>
-      <c r="D58" t="s">
-        <v>344</v>
-      </c>
-      <c r="V58" s="1">
-        <v>56</v>
-      </c>
-      <c r="X58" s="1">
-        <v>56</v>
-      </c>
-      <c r="AI58" s="1">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="59" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A59" s="1">
-        <v>58</v>
-      </c>
-      <c r="D59" t="s">
-        <v>346</v>
-      </c>
-      <c r="V59" s="1">
-        <v>57</v>
-      </c>
-      <c r="X59" s="1">
-        <v>57</v>
-      </c>
-      <c r="AI59" s="1">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="60" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A60" s="1">
-        <v>59</v>
-      </c>
-      <c r="D60" t="s">
-        <v>348</v>
-      </c>
-      <c r="V60" s="1">
-        <v>58</v>
-      </c>
-      <c r="X60" s="1">
-        <v>58</v>
-      </c>
-      <c r="AI60" s="1">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="61" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A61" s="1">
-        <v>60</v>
-      </c>
-      <c r="D61" t="s">
-        <v>350</v>
-      </c>
-      <c r="V61" s="1">
-        <v>59</v>
-      </c>
-      <c r="X61" s="1">
-        <v>59</v>
-      </c>
-      <c r="AI61" s="1">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="62" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A62" s="1">
-        <v>61</v>
-      </c>
-      <c r="D62" t="s">
-        <v>352</v>
-      </c>
-      <c r="V62" s="1">
-        <v>60</v>
-      </c>
-      <c r="X62" s="1">
-        <v>60</v>
-      </c>
-      <c r="AI62" s="1">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="63" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A63" s="1">
-        <v>62</v>
-      </c>
-      <c r="D63" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="64" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A64" s="1">
-        <v>63</v>
-      </c>
-      <c r="D64" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A65" s="1">
-        <v>64</v>
-      </c>
-      <c r="D65" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A66" s="1">
-        <v>65</v>
-      </c>
-      <c r="D66" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A67" s="1">
-        <v>66</v>
-      </c>
-      <c r="D67" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A68" s="1">
-        <v>67</v>
-      </c>
-      <c r="D68" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A69" s="1">
-        <v>68</v>
-      </c>
-      <c r="D69" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A70" s="1">
-        <v>69</v>
-      </c>
-      <c r="D70" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A71" s="1">
-        <v>70</v>
-      </c>
-      <c r="D71" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A72" s="1">
-        <v>71</v>
-      </c>
-      <c r="D72" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A73" s="1">
-        <v>72</v>
-      </c>
-      <c r="D73" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A74" s="1">
-        <v>73</v>
-      </c>
-      <c r="D74" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A75" s="1">
-        <v>74</v>
-      </c>
-      <c r="D75" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A76" s="1">
-        <v>75</v>
-      </c>
-      <c r="D76" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A77" s="1">
-        <v>76</v>
-      </c>
-      <c r="D77" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A78" s="1">
-        <v>77</v>
-      </c>
-      <c r="D78" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A79" s="1">
-        <v>78</v>
-      </c>
-      <c r="D79" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A80" s="1">
-        <v>79</v>
-      </c>
-      <c r="D80" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A81" s="1">
-        <v>80</v>
-      </c>
-      <c r="D81" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A82" s="1">
-        <v>81</v>
-      </c>
-      <c r="D82" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A83" s="1">
-        <v>82</v>
-      </c>
-      <c r="D83" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A84" s="1">
-        <v>83</v>
-      </c>
-      <c r="D84" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A85" s="1">
-        <v>84</v>
-      </c>
-      <c r="D85" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A86" s="1">
-        <v>85</v>
-      </c>
-      <c r="D86" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A87" s="1">
-        <v>86</v>
-      </c>
-      <c r="D87" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A88" s="1">
-        <v>87</v>
-      </c>
-      <c r="D88" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A89" s="1">
-        <v>88</v>
-      </c>
-      <c r="D89" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A90" s="1">
-        <v>89</v>
-      </c>
-      <c r="D90" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A91" s="1">
-        <v>90</v>
-      </c>
-      <c r="D91" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A92" s="1">
-        <v>91</v>
-      </c>
-      <c r="D92" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A93" s="1">
-        <v>92</v>
-      </c>
-      <c r="D93" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A94" s="1">
-        <v>93</v>
-      </c>
-      <c r="D94" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A95" s="1">
-        <v>94</v>
-      </c>
-      <c r="D95" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A96" s="1">
-        <v>95</v>
-      </c>
-      <c r="D96" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A97" s="1">
-        <v>96</v>
-      </c>
-      <c r="D97" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A98" s="1">
-        <v>97</v>
-      </c>
-      <c r="D98" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A99" s="1">
-        <v>98</v>
-      </c>
-      <c r="D99" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A100" s="1">
-        <v>99</v>
-      </c>
-      <c r="D100" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D101" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D102" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D103" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D104" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D105" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D106" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D107" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D108" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D109" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D110" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D111" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D112" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="113" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D113" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="114" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D114" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="115" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D115" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="116" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D116" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="117" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D117" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="118" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D118" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="119" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D119" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="120" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D120" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="121" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D121" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="122" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D122" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="123" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D123" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="124" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D124" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="125" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D125" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="126" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D126" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="127" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D127" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="128" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D128" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="129" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D129" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="130" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D130" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="131" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D131" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="132" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D132" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="133" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D133" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="134" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D134" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="135" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D135" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="136" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D136" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="137" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D137" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="138" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D138" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="139" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D139" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="140" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D140" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="141" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D141" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="142" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D142" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="143" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D143" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="144" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D144" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="145" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D145" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="146" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D146" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="147" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D147" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="148" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D148" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="149" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D149" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="150" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D150" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="151" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D151" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="152" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D152" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="153" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D153" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="154" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D154" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="155" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D155" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="156" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D156" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="157" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D157" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="158" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D158" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="159" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D159" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="160" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D160" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="161" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D161" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="162" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D162" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="163" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D163" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="164" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D164" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="165" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D165" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="166" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D166" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="167" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D167" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="168" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D168" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="169" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D169" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="170" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D170" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="171" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D171" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="172" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D172" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="173" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D173" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="174" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D174" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="175" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D175" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="176" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D176" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="177" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D177" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="178" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D178" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="179" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D179" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="180" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D180" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="181" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D181" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="182" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D182" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="183" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D183" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="184" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D184" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="185" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D185" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="186" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D186" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="187" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D187" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="188" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D188" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="189" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D189" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="190" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D190" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="191" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D191" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="192" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D192" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="193" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D193" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="194" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D194" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="195" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D195" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="196" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D196" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="197" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D197" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="198" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D198" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="199" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D199" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="200" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D200" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="201" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D201" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="202" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D202" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="203" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D203" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="204" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D204" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="205" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D205" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="206" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D206" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="207" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D207" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="208" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D208" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="209" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D209" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="210" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D210" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="211" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D211" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="212" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D212" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="213" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D213" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="214" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D214" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="215" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D215" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="216" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D216" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="217" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D217" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="218" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D218" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="219" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D219" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="220" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D220" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="221" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D221" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="222" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D222" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="223" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D223" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="224" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D224" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="225" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D225" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="226" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D226" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="227" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D227" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="228" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D228" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="229" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D229" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="230" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D230" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="231" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D231" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="232" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D232" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="233" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D233" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="234" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D234" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="235" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D235" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="236" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D236" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="237" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D237" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="238" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D238" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="239" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D239" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="240" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D240" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="241" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D241" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="242" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D242" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="243" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D243" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="244" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D244" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="245" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D245" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="246" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D246" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="247" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D247" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="248" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D248" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="249" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D249" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="250" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D250" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="251" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D251" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="252" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D252" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="253" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D253" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="254" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D254" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="255" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D255" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="256" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D256" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="257" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D257" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="258" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D258" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="259" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D259" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="260" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D260" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="261" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D261" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="262" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D262" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="263" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D263" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="264" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D264" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="265" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D265" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="266" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D266" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="267" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D267" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="268" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D268" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="269" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D269" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="270" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D270" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="271" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D271" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="272" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D272" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="273" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D273" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="274" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D274" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="275" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D275" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="276" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D276" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="277" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D277" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="278" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D278" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="279" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D279" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="280" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D280" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="281" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D281" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="282" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D282" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="283" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D283" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="284" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D284" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="285" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D285" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="286" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D286" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="287" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D287" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="288" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D288" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="289" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D289" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="290" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D290" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="291" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D291" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="292" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D292" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="293" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D293" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="294" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D294" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="295" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D295" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="296" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D296" t="s">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="297" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D297" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="298" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D298" t="s">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="299" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D299" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="300" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D300" t="s">
-        <v>614</v>
-      </c>
-    </row>
-    <row r="301" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D301" t="s">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="302" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D302" t="s">
-        <v>616</v>
-      </c>
-    </row>
-    <row r="303" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D303" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="304" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D304" t="s">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="305" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D305" t="s">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="306" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D306" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="307" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D307" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="308" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D308" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="309" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D309" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="310" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D310" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="311" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D311" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="312" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D312" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="313" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D313" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="314" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D314" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="315" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D315" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="316" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D316" t="s">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="317" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D317" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="318" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D318" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="319" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D319" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="320" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D320" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="321" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D321" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="322" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D322" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="323" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D323" t="s">
-        <v>637</v>
-      </c>
-    </row>
-    <row r="324" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D324" t="s">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="325" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D325" t="s">
-        <v>639</v>
-      </c>
-    </row>
-    <row r="326" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D326" t="s">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="327" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D327" t="s">
-        <v>641</v>
-      </c>
-    </row>
-    <row r="328" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D328" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="329" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D329" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="330" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D330" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="331" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D331" t="s">
-        <v>645</v>
-      </c>
-    </row>
-    <row r="332" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D332" t="s">
-        <v>646</v>
-      </c>
-    </row>
-    <row r="333" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D333" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="334" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D334" t="s">
-        <v>648</v>
-      </c>
-    </row>
-    <row r="335" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D335" t="s">
-        <v>649</v>
-      </c>
-    </row>
-    <row r="336" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D336" t="s">
-        <v>650</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:AT336"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
+      <selection activeCell="AJ5" sqref="AJ5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6429,7 +2803,7 @@
         <v>665</v>
       </c>
       <c r="K1" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="L1" t="s">
         <v>667</v>
@@ -10452,14 +6826,16 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:CN2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -11117,7 +7493,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>

</xml_diff>